<commit_message>
changed any target values of 0 to 1e-7 to avoid dividing by 0 in gof function
</commit_message>
<xml_diff>
--- a/Data/model_inputs.xlsx
+++ b/Data/model_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/briannalauren/Desktop/Columbia_RA/lynch_syndrome/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10DD5AC-FCA8-C247-B409-2F4D84D7B142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277FE499-ACB9-174F-93D1-C6ACD68F8FC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" firstSheet="15" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MLH1" sheetId="1" r:id="rId1"/>
@@ -548,19 +548,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -971,7 +965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -1714,7 +1708,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1732,7 +1726,8 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f>0.0000001</f>
+        <v>9.9999999999999995E-8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1961,7 +1956,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1979,7 +1974,8 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f>0.0000001</f>
+        <v>9.9999999999999995E-8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2168,7 +2164,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2186,7 +2182,8 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f>0.0000001</f>
+        <v>9.9999999999999995E-8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2383,7 +2380,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2401,7 +2398,8 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f>0.0000001</f>
+        <v>9.9999999999999995E-8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2598,7 +2596,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2616,7 +2614,8 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f>0.0000001</f>
+        <v>9.9999999999999995E-8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2765,7 +2764,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2783,7 +2782,8 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f>0.0000001</f>
+        <v>9.9999999999999995E-8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2988,7 +2988,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3006,7 +3006,8 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f>0.0000001</f>
+        <v>9.9999999999999995E-8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3405,7 +3406,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3423,7 +3424,8 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f>0.0000001</f>
+        <v>9.9999999999999995E-8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3595,8 +3597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CCD98A-C0EB-4C6C-9836-93985E235FAD}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4117,10 +4119,13 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -4141,8 +4146,8 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <f>AVERAGE(E2,F2)</f>
-        <v>0</v>
+        <f>0.0000001</f>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -4297,7 +4302,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4321,8 +4326,8 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <f>AVERAGE(E2,F2)</f>
-        <v>0</v>
+        <f>0.0000001</f>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="E2">
         <v>0</v>

</xml_diff>